<commit_message>
Smoothed transitions and performed stress testing
</commit_message>
<xml_diff>
--- a/documentation/project2_worklog.xlsx
+++ b/documentation/project2_worklog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kansas-my.sharepoint.com/personal/l495p005_home_ku_edu/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Landon\Desktop\EECS 581\Project_2\EECS-581-Project-2\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1EFFF341-288B-4F8F-AEB8-D3299E47EBD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA60CAF-953D-42D9-8EE6-8EF2E3DB8944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{016D3725-BEF8-41FD-9F88-E735BA5F306E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>Log Number</t>
   </si>
@@ -108,13 +108,34 @@
   </si>
   <si>
     <t>Scanned through code. Helped Kai resolve conflicts. Started updating the worklog file. Planning to look at medium difficulty</t>
+  </si>
+  <si>
+    <t>Landon, Aiden, Andrew</t>
+  </si>
+  <si>
+    <t>Added all comments to ai shooting behavior code</t>
+  </si>
+  <si>
+    <t>Discussed ship difficulty logic</t>
+  </si>
+  <si>
+    <t>Overwrote get_input in AI class to just return coordinate from aiTurn. Added gameloop logic so that you can actually play against AI now. Seems that at least easy mode is working, haven't had a chance to test other modes</t>
+  </si>
+  <si>
+    <t>Changed AI class to inherit Player so that functions aren't being recreated. Overwrote some functions from Player and GameObject to fit the AI better. Ship placement logic may be done but hasn't been tested and isn't optimized since it's always randomizing without knowledge of previous ship placements or board boundaries and instead error checks each time. Started to modify __take_turn() to take in coordinates from aiTurn but still needs a lot of attention. Waiting for Andrew to push comments on aiTurn function before I start messing with it so that merge conflicts are avoided</t>
+  </si>
+  <si>
+    <t>Cleaned some more code and implemented medium and hard difficulty for the AI</t>
+  </si>
+  <si>
+    <t>Made better transitions between Player -&gt; Player and Player -&gt; AI based off of input buffer instead of waiting. Spent a lot of time stress testing with different combinations of AI difficulties, ship amounts, ship directions, and super shot. Updated worklog to be up to date.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -498,18 +519,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD21634D-05D0-4FC5-8519-ABDDC6FAB35E}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -529,7 +550,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -549,7 +570,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -569,7 +590,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -589,7 +610,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -609,7 +630,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -629,7 +650,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -649,7 +670,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -669,7 +690,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -689,7 +710,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -709,7 +730,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -729,79 +750,181 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="3:3">
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="3:3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="2">
+        <v>45562</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>40</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="2">
+        <v>45563</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="2">
+        <v>45563</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2">
+        <v>45563</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="2">
+        <v>45563</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>30</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="2">
+        <v>45563</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="3:3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="3:3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="3:3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="3:3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="3:3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="3:3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="3:3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="3:3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="3:3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="3:3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="3:3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C29" s="2"/>
     </row>
-    <row r="30" spans="3:3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C30" s="2"/>
     </row>
-    <row r="31" spans="3:3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="3:3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C32" s="2"/>
     </row>
-    <row r="33" spans="3:3">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C33" s="2"/>
     </row>
-    <row r="34" spans="3:3">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C34" s="2"/>
     </row>
-    <row r="35" spans="3:3">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C35" s="2"/>
     </row>
-    <row r="36" spans="3:3">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C36" s="2"/>
     </row>
   </sheetData>
@@ -811,23 +934,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5a59c2ea-6c19-4a10-8ede-52039d141628" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100719F37FE48B01A409F32F6E741AFC455" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d86eaf982ccaec4dc1560e6acaea1cbb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5a59c2ea-6c19-4a10-8ede-52039d141628" xmlns:ns4="ed461fce-0a4d-4919-9b1a-aacc4f02b5ed" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c0de1d84ec3d20b6822b8daf3c3b0c0c" ns3:_="" ns4:_="">
     <xsd:import namespace="5a59c2ea-6c19-4a10-8ede-52039d141628"/>
@@ -1036,14 +1142,56 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5a59c2ea-6c19-4a10-8ede-52039d141628" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2621EC10-4799-4EF7-8A1D-5D359CF7A094}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96372B58-5A9A-470A-BF06-01A11DFFCB26}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="5a59c2ea-6c19-4a10-8ede-52039d141628"/>
+    <ds:schemaRef ds:uri="ed461fce-0a4d-4919-9b1a-aacc4f02b5ed"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9007B3CB-C24B-48DB-9B05-ADDED9763589}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9007B3CB-C24B-48DB-9B05-ADDED9763589}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96372B58-5A9A-470A-BF06-01A11DFFCB26}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2621EC10-4799-4EF7-8A1D-5D359CF7A094}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5a59c2ea-6c19-4a10-8ede-52039d141628"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>